<commit_message>
Przejście na funkcje asynchroniczne
</commit_message>
<xml_diff>
--- a/PLC_SIEMENS/Alarmy.xlsx
+++ b/PLC_SIEMENS/Alarmy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krzys\OneDrive\Pulpit\UMG\_Praca inżynierska\SCADA\PLC_SIEMENS\PLC_SIEMENS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F655B7-A29C-4349-9E56-554E555A745B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC860DA-CD8B-4517-8B35-6541843C1977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1635" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31005" yWindow="2580" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alarmy" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="393">
   <si>
     <t>ID</t>
   </si>
@@ -1209,6 +1209,9 @@
   </si>
   <si>
     <t>2024.01.14 21:35</t>
+  </si>
+  <si>
+    <t>niedziela, 25 lutego 2024 22:33:36</t>
   </si>
 </sst>
 </file>
@@ -1634,7 +1637,7 @@
         <v>389</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>